<commit_message>
Revised the documentation and comments Use csv format for the incident files
</commit_message>
<xml_diff>
--- a/out/00 factors.xlsx
+++ b/out/00 factors.xlsx
@@ -503,16 +503,16 @@
         <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>5062.013458560402</v>
+        <v>5086.153335856128</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9015337936114683</v>
+        <v>0.8540265712417093</v>
       </c>
       <c r="I2" t="n">
-        <v>0.04905457279069363</v>
+        <v>0.04997149770573032</v>
       </c>
     </row>
     <row r="3">
@@ -538,16 +538,16 @@
         <v>16</v>
       </c>
       <c r="F3" t="n">
-        <v>1201.084055545566</v>
+        <v>1204.914932712188</v>
       </c>
       <c r="G3" t="n">
-        <v>9.572574959585271e-247</v>
+        <v>1.439258204408449e-247</v>
       </c>
       <c r="H3" t="n">
-        <v>0.04199055645104691</v>
+        <v>0.0675069979266494</v>
       </c>
       <c r="I3" t="n">
-        <v>0.02656152611675559</v>
+        <v>0.02146796566642512</v>
       </c>
     </row>
     <row r="4">
@@ -573,16 +573,16 @@
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>220.5158252870746</v>
+        <v>220.8241972240276</v>
       </c>
       <c r="G4" t="n">
-        <v>6.980226719986232e-50</v>
+        <v>5.978698520033615e-50</v>
       </c>
       <c r="H4" t="n">
-        <v>0.02509623056070723</v>
+        <v>0.03113305331997251</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01880236057734017</v>
+        <v>0.01358754557154232</v>
       </c>
     </row>
     <row r="5">
@@ -608,16 +608,16 @@
         <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7859219645519846</v>
+        <v>0.8883290064550426</v>
       </c>
       <c r="G5" t="n">
-        <v>0.375336089387886</v>
+        <v>0.3459305333140232</v>
       </c>
       <c r="H5" t="n">
-        <v>0.007007616490164711</v>
+        <v>0.00492061072439518</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0111501935098194</v>
+        <v>0.002660039725387586</v>
       </c>
     </row>
     <row r="6">
@@ -643,16 +643,16 @@
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>85.03539735886675</v>
+        <v>86.00805738538253</v>
       </c>
       <c r="G6" t="n">
-        <v>2.930712052604616e-20</v>
+        <v>1.792039823210119e-20</v>
       </c>
       <c r="H6" t="n">
-        <v>0.005773965052043</v>
+        <v>0.002000261713705436</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01078907443846973</v>
+        <v>0.002567947345023552</v>
       </c>
     </row>
     <row r="7">
@@ -678,26 +678,26 @@
         <v>16</v>
       </c>
       <c r="F7" t="n">
-        <v>384.3171526993451</v>
+        <v>392.3837685207457</v>
       </c>
       <c r="G7" t="n">
-        <v>1.358657888241235e-72</v>
+        <v>2.752934587762642e-74</v>
       </c>
       <c r="H7" t="n">
-        <v>0.006951365941291337</v>
+        <v>0.01301928421089169</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00188231226842886</v>
+        <v>0.00237484453601966</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>has_knowledge_article</t>
+          <t>self_service</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -713,15 +713,17 @@
         <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>34.30570374311844</v>
+        <v>42.314501917315</v>
       </c>
       <c r="G8" t="n">
-        <v>4.709993648472096e-09</v>
+        <v>7.771416267429973e-11</v>
       </c>
       <c r="H8" t="n">
-        <v>0.005488917236315931</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
+        <v>0.0003918017624877692</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0007551729345986052</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -746,13 +748,13 @@
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>116.0908939128296</v>
+        <v>116.6857017813586</v>
       </c>
       <c r="G9" t="n">
-        <v>4.540043543283562e-27</v>
+        <v>3.363625883314413e-27</v>
       </c>
       <c r="H9" t="n">
-        <v>0.002531471778483367</v>
+        <v>0.02110987240302388</v>
       </c>
       <c r="I9" t="inlineStr"/>
     </row>
@@ -779,24 +781,24 @@
         <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>908.9557835042174</v>
+        <v>915.4726472302203</v>
       </c>
       <c r="G10" t="n">
-        <v>1.109051363170596e-199</v>
+        <v>4.248980687842385e-201</v>
       </c>
       <c r="H10" t="n">
-        <v>0.002124437843850688</v>
+        <v>0.003545907502174473</v>
       </c>
       <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>self_service</t>
+          <t>has_knowledge_article</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -812,13 +814,13 @@
         <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>40.67857666800625</v>
+        <v>34.81280277953115</v>
       </c>
       <c r="G11" t="n">
-        <v>1.794437343421407e-10</v>
+        <v>3.629786486834646e-09</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0008014904885535787</v>
+        <v>0.002345639194990277</v>
       </c>
       <c r="I11" t="inlineStr"/>
     </row>
@@ -845,13 +847,13 @@
         <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>109.2587322909771</v>
+        <v>109.391853707005</v>
       </c>
       <c r="G12" t="n">
-        <v>1.424268573634559e-25</v>
+        <v>1.331757529725758e-25</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0007001545460747457</v>
+        <v>0</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
@@ -878,10 +880,10 @@
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>30.01301901709297</v>
+        <v>30.0312876065441</v>
       </c>
       <c r="G13" t="n">
-        <v>4.291552891289624e-08</v>
+        <v>4.251311960370145e-08</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -911,10 +913,10 @@
         <v>2</v>
       </c>
       <c r="F14" t="n">
-        <v>20.72392705923381</v>
+        <v>21.56381917347364</v>
       </c>
       <c r="G14" t="n">
-        <v>5.30489710067143e-06</v>
+        <v>3.422476790024476e-06</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -944,10 +946,10 @@
         <v>2</v>
       </c>
       <c r="F15" t="n">
-        <v>14.97738401036684</v>
+        <v>15.28524034640144</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0001088074403523893</v>
+        <v>9.243595384270451e-05</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -977,10 +979,10 @@
         <v>2</v>
       </c>
       <c r="F16" t="n">
-        <v>3.755177606479185</v>
+        <v>3.540962606063545</v>
       </c>
       <c r="G16" t="n">
-        <v>0.05264420264064077</v>
+        <v>0.05987070582593627</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1005,13 +1007,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>1981</v>
+        <v>1988</v>
       </c>
       <c r="F17" t="n">
-        <v>2660.683781866036</v>
+        <v>2681.182401149468</v>
       </c>
       <c r="G17" t="n">
-        <v>6.281977847913644e-23</v>
+        <v>1.250721961446571e-23</v>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -1034,13 +1036,13 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="F18" t="n">
-        <v>1822.524598921105</v>
+        <v>1824.123930449769</v>
       </c>
       <c r="G18" t="n">
-        <v>9.202799494861961e-76</v>
+        <v>2.858346425893734e-75</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
@@ -1063,13 +1065,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F19" t="n">
-        <v>757.0477081279878</v>
+        <v>757.5341707421819</v>
       </c>
       <c r="G19" t="n">
-        <v>1.055341826075107e-94</v>
+        <v>2.201367192346436e-94</v>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
@@ -1095,10 +1097,10 @@
         <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>334.2336581984052</v>
+        <v>335.8134709170386</v>
       </c>
       <c r="G20" t="n">
-        <v>1.400057343459844e-66</v>
+        <v>6.459790618508831e-67</v>
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
@@ -1124,10 +1126,10 @@
         <v>11</v>
       </c>
       <c r="F21" t="n">
-        <v>104.9694982966936</v>
+        <v>103.315517062819</v>
       </c>
       <c r="G21" t="n">
-        <v>5.492938861828806e-18</v>
+        <v>1.180107952614957e-17</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
@@ -1153,10 +1155,10 @@
         <v>5</v>
       </c>
       <c r="F22" t="n">
-        <v>73.82325109790953</v>
+        <v>75.24537910926617</v>
       </c>
       <c r="G22" t="n">
-        <v>3.533923241743454e-15</v>
+        <v>1.76813754184472e-15</v>
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
@@ -1182,10 +1184,10 @@
         <v>11</v>
       </c>
       <c r="F23" t="n">
-        <v>52.28655870110554</v>
+        <v>53.02979898947834</v>
       </c>
       <c r="G23" t="n">
-        <v>1.009852580679422e-07</v>
+        <v>7.351678343089048e-08</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
@@ -1211,10 +1213,10 @@
         <v>4</v>
       </c>
       <c r="F24" t="n">
-        <v>25.10952190195545</v>
+        <v>23.80406556053098</v>
       </c>
       <c r="G24" t="n">
-        <v>1.464738759557574e-05</v>
+        <v>2.744679293689399e-05</v>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
@@ -1240,10 +1242,10 @@
         <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2430458325876041</v>
+        <v>0.2463471129800019</v>
       </c>
       <c r="G25" t="n">
-        <v>0.6220148571644246</v>
+        <v>0.6196590139590284</v>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>

</xml_diff>

<commit_message>
Updated Incident dissatisfaction analysis doc Revied output file in support of analysis
</commit_message>
<xml_diff>
--- a/out/00 factors.xlsx
+++ b/out/00 factors.xlsx
@@ -503,16 +503,16 @@
         <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>5084.708078551253</v>
+        <v>5092.189991138204</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9174228422786094</v>
+        <v>0.8281579550181661</v>
       </c>
       <c r="I2" t="n">
-        <v>0.04992103286120007</v>
+        <v>0.0500700922614565</v>
       </c>
     </row>
     <row r="3">
@@ -531,23 +531,23 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>int32</t>
         </is>
       </c>
       <c r="E3" t="n">
         <v>16</v>
       </c>
       <c r="F3" t="n">
-        <v>1219.647613092101</v>
+        <v>1257.180129695942</v>
       </c>
       <c r="G3" t="n">
-        <v>9.845271300420358e-251</v>
+        <v>8.48333177665778e-259</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0475366043163568</v>
+        <v>0.07588495907475241</v>
       </c>
       <c r="I3" t="n">
-        <v>0.02857560401052137</v>
+        <v>0.02902936262715672</v>
       </c>
     </row>
     <row r="4">
@@ -573,26 +573,26 @@
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>229.8268714047051</v>
+        <v>228.1239131884054</v>
       </c>
       <c r="G4" t="n">
-        <v>6.50278065057951e-52</v>
+        <v>1.529300995221543e-51</v>
       </c>
       <c r="H4" t="n">
-        <v>0.009510591851889585</v>
+        <v>0.03604976869833777</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0146107968157409</v>
+        <v>0.02064419431967895</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>caller_is_employee</t>
+          <t>close_code_Information Provided / Training</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -601,33 +601,33 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>uint8</t>
         </is>
       </c>
       <c r="E5" t="n">
         <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>86.92340326302833</v>
+        <v>0.4465915044955309</v>
       </c>
       <c r="G5" t="n">
-        <v>1.128065634331642e-20</v>
+        <v>0.5039580546878374</v>
       </c>
       <c r="H5" t="n">
-        <v>0.005613102857774587</v>
+        <v>0.01941880190963343</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01350479925007277</v>
+        <v>0.01373907580264028</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>close_code_Information Provided / Training</t>
+          <t>caller_is_employee</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -636,23 +636,23 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>uint8</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6803916324121152</v>
+        <v>83.80762975576576</v>
       </c>
       <c r="G6" t="n">
-        <v>0.409451899540245</v>
+        <v>5.453393717197261e-20</v>
       </c>
       <c r="H6" t="n">
-        <v>0.002420080664796069</v>
+        <v>0.01548728146001643</v>
       </c>
       <c r="I6" t="n">
-        <v>0.007915165728451565</v>
+        <v>0.01265844223435578</v>
       </c>
     </row>
     <row r="7">
@@ -678,26 +678,26 @@
         <v>16</v>
       </c>
       <c r="F7" t="n">
-        <v>397.6277361644023</v>
+        <v>412.5782679072584</v>
       </c>
       <c r="G7" t="n">
-        <v>2.179542287274404e-75</v>
+        <v>1.568792188957606e-78</v>
       </c>
       <c r="H7" t="n">
-        <v>0.006159906947999291</v>
+        <v>0.01446973926677739</v>
       </c>
       <c r="I7" t="n">
-        <v>0.005004185680185222</v>
+        <v>0.003868025272335054</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>close_code_Reboot / Restart</t>
+          <t>self_service</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -706,33 +706,33 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>uint8</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="E8" t="n">
         <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>31.6108223697001</v>
+        <v>37.13716479571343</v>
       </c>
       <c r="G8" t="n">
-        <v>1.88376839400601e-08</v>
+        <v>1.101050928906596e-09</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0001776015571267704</v>
+        <v>0.0007380035089618395</v>
       </c>
       <c r="I8" t="n">
-        <v>0.000485078026207536</v>
+        <v>0.001056843058807017</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>priority_is_4</t>
+          <t>close_code_Reboot / Restart</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -741,33 +741,33 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>uint8</t>
         </is>
       </c>
       <c r="E9" t="n">
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>109.1455868090539</v>
+        <v>31.37291815963541</v>
       </c>
       <c r="G9" t="n">
-        <v>1.507933417490376e-25</v>
+        <v>2.129303318114019e-08</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0002100012995132499</v>
+        <v>0.002220262839033624</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0003510411609796982</v>
+        <v>0.0004798641183796776</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>close_code_Security Modification</t>
+          <t>has_knowledge_article</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -776,33 +776,31 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>uint8</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="E10" t="n">
         <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>21.61467690125398</v>
+        <v>31.16121867954963</v>
       </c>
       <c r="G10" t="n">
-        <v>3.332916503252091e-06</v>
+        <v>2.374630093836708e-08</v>
       </c>
       <c r="H10" t="n">
-        <v>4.138755406552182e-05</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.0001435126986766982</v>
-      </c>
+        <v>0.003907921314528814</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>close_code_Data Correction</t>
+          <t>sla_breached</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -811,31 +809,31 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>uint8</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="E11" t="n">
         <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>120.4352571348047</v>
+        <v>942.0908075192066</v>
       </c>
       <c r="G11" t="n">
-        <v>5.079785285019881e-28</v>
+        <v>6.950472456256092e-207</v>
       </c>
       <c r="H11" t="n">
-        <v>0.006221864429556639</v>
+        <v>0.003103394089759474</v>
       </c>
       <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>sla_breached</t>
+          <t>priority_is_4</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -851,24 +849,24 @@
         <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>900.9033892294275</v>
+        <v>102.8065078049167</v>
       </c>
       <c r="G12" t="n">
-        <v>6.243597253286266e-198</v>
+        <v>3.69533624371533e-24</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00232410098489939</v>
+        <v>0.0005619128200327663</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>has_knowledge_article</t>
+          <t>close_code_Data Correction</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -877,31 +875,31 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>uint8</t>
         </is>
       </c>
       <c r="E13" t="n">
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>35.06926536617871</v>
+        <v>118.3582804409064</v>
       </c>
       <c r="G13" t="n">
-        <v>3.181833609544766e-09</v>
+        <v>1.447344220452242e-27</v>
       </c>
       <c r="H13" t="n">
-        <v>0.001377551787330197</v>
+        <v>0</v>
       </c>
       <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>self_service</t>
+          <t>close_code_Security Modification</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -910,20 +908,20 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>uint8</t>
         </is>
       </c>
       <c r="E14" t="n">
         <v>2</v>
       </c>
       <c r="F14" t="n">
-        <v>42.23504842217222</v>
+        <v>24.57884854687371</v>
       </c>
       <c r="G14" t="n">
-        <v>8.093643014044539e-11</v>
+        <v>7.133040263298417e-07</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0009843634700822583</v>
+        <v>0</v>
       </c>
       <c r="I14" t="inlineStr"/>
     </row>
@@ -950,10 +948,10 @@
         <v>2</v>
       </c>
       <c r="F15" t="n">
-        <v>15.27141667140958</v>
+        <v>10.21101912764689</v>
       </c>
       <c r="G15" t="n">
-        <v>9.311492256008624e-05</v>
+        <v>0.001396040065543618</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -983,10 +981,10 @@
         <v>2</v>
       </c>
       <c r="F16" t="n">
-        <v>3.486221407548221</v>
+        <v>3.745106367170496</v>
       </c>
       <c r="G16" t="n">
-        <v>0.06188167984311064</v>
+        <v>0.05296235631384372</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1011,13 +1009,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="F17" t="n">
-        <v>2706.423120236372</v>
+        <v>2707.88430286518</v>
       </c>
       <c r="G17" t="n">
-        <v>3.767079800315948e-25</v>
+        <v>3.618990377525164e-25</v>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -1043,10 +1041,10 @@
         <v>840</v>
       </c>
       <c r="F18" t="n">
-        <v>1846.25373189093</v>
+        <v>1879.114990546355</v>
       </c>
       <c r="G18" t="n">
-        <v>1.503960617385468e-77</v>
+        <v>1.745139109679028e-81</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
@@ -1069,13 +1067,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F19" t="n">
-        <v>765.3432532648524</v>
+        <v>810.4490601548114</v>
       </c>
       <c r="G19" t="n">
-        <v>2.04984278226451e-95</v>
+        <v>1.620596205769993e-102</v>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
@@ -1101,10 +1099,10 @@
         <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>346.602411731557</v>
+        <v>341.2105583346715</v>
       </c>
       <c r="G20" t="n">
-        <v>3.275009766285184e-69</v>
+        <v>4.59564601261427e-68</v>
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
@@ -1130,10 +1128,10 @@
         <v>11</v>
       </c>
       <c r="F21" t="n">
-        <v>107.5382347212224</v>
+        <v>103.4231650211193</v>
       </c>
       <c r="G21" t="n">
-        <v>1.67182232173552e-18</v>
+        <v>1.122843000026662e-17</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
@@ -1159,10 +1157,10 @@
         <v>5</v>
       </c>
       <c r="F22" t="n">
-        <v>74.25580520776305</v>
+        <v>69.82738917504001</v>
       </c>
       <c r="G22" t="n">
-        <v>2.862857228083405e-15</v>
+        <v>2.468511659415333e-14</v>
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
@@ -1185,13 +1183,13 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>52.67135297523705</v>
+        <v>55.67919274080439</v>
       </c>
       <c r="G23" t="n">
-        <v>8.568760406818492e-08</v>
+        <v>9.038441793712736e-09</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
@@ -1217,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="F24" t="n">
-        <v>21.93541781183875</v>
+        <v>21.06684547225731</v>
       </c>
       <c r="G24" t="n">
-        <v>6.728089110469279e-05</v>
+        <v>0.0001019640655452652</v>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
@@ -1246,10 +1244,10 @@
         <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1860382191881642</v>
+        <v>0.1937002312628119</v>
       </c>
       <c r="G25" t="n">
-        <v>0.666234633972506</v>
+        <v>0.6598546263428959</v>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>

</xml_diff>